<commit_message>
add ability to remove gridlines, set other properties
</commit_message>
<xml_diff>
--- a/test/out/example3.xlsx
+++ b/test/out/example3.xlsx
@@ -15,25 +15,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>I am title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>WCenter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WRType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Eng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WorkNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreationTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -41,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="宋体"/>
@@ -49,8 +57,17 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -60,13 +77,33 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -75,8 +112,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="0" horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -373,46 +413,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" zoomScaleNormal="50" zoomScale="50"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="40" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1"/>
-      <c r="G1"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2"/>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1.5</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>2.5</v>
-      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2"/>
@@ -542,6 +587,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="200" verticalDpi="200"/>
 </worksheet>
 </file>
</xml_diff>